<commit_message>
final pre-test-rig animation sketches
</commit_message>
<xml_diff>
--- a/animations/2-sparkle-a.xlsx
+++ b/animations/2-sparkle-a.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10410"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:11_{818CA356-4044-764F-BCAE-306ACB787E83}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:11_{2B01B0BC-047F-E54A-BC44-CD08AD323A34}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="660" yWindow="460" windowWidth="49220" windowHeight="28340" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="50240" windowHeight="28340" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -29,13 +29,68 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF63449F"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF7B58BF"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF936BDF"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFAB7FFF"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFE8DDFF"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF8B65D4"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFB791FF"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFD0B7FF"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -50,14 +105,92 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="1">
+  <dxfs count="11">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -348,10 +481,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AT2"/>
+  <dimension ref="A1:AT46"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="400" zoomScaleNormal="400" workbookViewId="0">
-      <selection activeCell="H4" sqref="H4"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="400" zoomScaleNormal="400" workbookViewId="0">
+      <selection activeCell="J30" sqref="J30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -530,9 +663,1070 @@
         <v>8</v>
       </c>
     </row>
+    <row r="3" spans="1:46" x14ac:dyDescent="0.2">
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="C3">
+        <v>2</v>
+      </c>
+      <c r="D3">
+        <v>3</v>
+      </c>
+      <c r="E3">
+        <v>4</v>
+      </c>
+      <c r="F3">
+        <v>5</v>
+      </c>
+      <c r="G3">
+        <v>6</v>
+      </c>
+      <c r="H3">
+        <v>7</v>
+      </c>
+      <c r="I3">
+        <v>8</v>
+      </c>
+      <c r="J3">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:46" x14ac:dyDescent="0.2">
+      <c r="C4">
+        <v>1</v>
+      </c>
+      <c r="D4">
+        <v>2</v>
+      </c>
+      <c r="E4">
+        <v>3</v>
+      </c>
+      <c r="F4">
+        <v>4</v>
+      </c>
+      <c r="G4">
+        <v>5</v>
+      </c>
+      <c r="H4">
+        <v>6</v>
+      </c>
+      <c r="I4">
+        <v>7</v>
+      </c>
+      <c r="J4">
+        <v>8</v>
+      </c>
+      <c r="K4">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:46" x14ac:dyDescent="0.2">
+      <c r="E5">
+        <v>1</v>
+      </c>
+      <c r="F5">
+        <v>2</v>
+      </c>
+      <c r="G5">
+        <v>3</v>
+      </c>
+      <c r="H5">
+        <v>4</v>
+      </c>
+      <c r="I5">
+        <v>5</v>
+      </c>
+      <c r="J5">
+        <v>6</v>
+      </c>
+      <c r="K5">
+        <v>7</v>
+      </c>
+      <c r="L5">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:46" x14ac:dyDescent="0.2">
+      <c r="F6">
+        <v>1</v>
+      </c>
+      <c r="G6">
+        <v>2</v>
+      </c>
+      <c r="H6">
+        <v>3</v>
+      </c>
+      <c r="I6">
+        <v>4</v>
+      </c>
+      <c r="J6">
+        <v>5</v>
+      </c>
+      <c r="K6">
+        <v>6</v>
+      </c>
+      <c r="L6">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:46" x14ac:dyDescent="0.2">
+      <c r="H7">
+        <v>1</v>
+      </c>
+      <c r="I7">
+        <v>2</v>
+      </c>
+      <c r="J7">
+        <v>3</v>
+      </c>
+      <c r="K7">
+        <v>4</v>
+      </c>
+      <c r="L7">
+        <v>5</v>
+      </c>
+      <c r="M7">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:46" x14ac:dyDescent="0.2">
+      <c r="I8">
+        <v>1</v>
+      </c>
+      <c r="J8">
+        <v>2</v>
+      </c>
+      <c r="K8">
+        <v>3</v>
+      </c>
+      <c r="L8">
+        <v>4</v>
+      </c>
+      <c r="M8">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:46" x14ac:dyDescent="0.2">
+      <c r="K9">
+        <v>1</v>
+      </c>
+      <c r="L9">
+        <v>2</v>
+      </c>
+      <c r="M9" s="4">
+        <v>3</v>
+      </c>
+      <c r="N9" s="4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:46" x14ac:dyDescent="0.2">
+      <c r="L10">
+        <v>1</v>
+      </c>
+      <c r="M10" s="3">
+        <v>2</v>
+      </c>
+      <c r="N10" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:46" x14ac:dyDescent="0.2">
+      <c r="M11" s="2"/>
+      <c r="N11" s="2">
+        <v>1</v>
+      </c>
+      <c r="O11" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:46" x14ac:dyDescent="0.2">
+      <c r="M12" s="2"/>
+      <c r="N12" s="2"/>
+      <c r="O12" s="2"/>
+    </row>
+    <row r="13" spans="1:46" x14ac:dyDescent="0.2">
+      <c r="M13" s="2"/>
+      <c r="N13" s="2"/>
+      <c r="O13" s="2"/>
+      <c r="Q13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:46" x14ac:dyDescent="0.2">
+      <c r="M14" s="2"/>
+      <c r="N14" s="2"/>
+      <c r="O14" s="2"/>
+      <c r="Q14">
+        <v>1</v>
+      </c>
+      <c r="T14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:46" x14ac:dyDescent="0.2">
+      <c r="M15" s="2"/>
+      <c r="N15" s="2">
+        <v>1</v>
+      </c>
+      <c r="O15" s="2"/>
+      <c r="Q15">
+        <v>2</v>
+      </c>
+      <c r="R15">
+        <v>1</v>
+      </c>
+      <c r="T15">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:46" x14ac:dyDescent="0.2">
+      <c r="M16" s="2"/>
+      <c r="N16" s="2">
+        <v>1</v>
+      </c>
+      <c r="O16" s="2"/>
+      <c r="Q16">
+        <v>1</v>
+      </c>
+      <c r="T16">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="17" spans="8:23" x14ac:dyDescent="0.2">
+      <c r="M17" s="2"/>
+      <c r="N17" s="2">
+        <v>2</v>
+      </c>
+      <c r="O17" s="2">
+        <v>1</v>
+      </c>
+      <c r="R17">
+        <v>1</v>
+      </c>
+      <c r="T17">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="18" spans="8:23" x14ac:dyDescent="0.2">
+      <c r="N18">
+        <v>3</v>
+      </c>
+      <c r="O18">
+        <v>1</v>
+      </c>
+      <c r="Q18">
+        <v>1</v>
+      </c>
+      <c r="R18">
+        <v>1</v>
+      </c>
+      <c r="T18">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="19" spans="8:23" x14ac:dyDescent="0.2">
+      <c r="N19">
+        <v>4</v>
+      </c>
+      <c r="O19">
+        <v>2</v>
+      </c>
+      <c r="P19">
+        <v>1</v>
+      </c>
+      <c r="Q19">
+        <v>2</v>
+      </c>
+      <c r="R19">
+        <v>2</v>
+      </c>
+      <c r="T19">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="20" spans="8:23" x14ac:dyDescent="0.2">
+      <c r="N20">
+        <v>5</v>
+      </c>
+      <c r="O20" s="2">
+        <v>1</v>
+      </c>
+      <c r="P20">
+        <v>2</v>
+      </c>
+      <c r="Q20">
+        <v>1</v>
+      </c>
+      <c r="R20">
+        <v>3</v>
+      </c>
+      <c r="T20">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="22" spans="8:23" x14ac:dyDescent="0.2">
+      <c r="L22">
+        <v>1</v>
+      </c>
+      <c r="N22">
+        <v>7</v>
+      </c>
+      <c r="O22">
+        <v>1</v>
+      </c>
+      <c r="P22">
+        <v>4</v>
+      </c>
+      <c r="Q22">
+        <v>1</v>
+      </c>
+      <c r="R22">
+        <v>4</v>
+      </c>
+      <c r="T22">
+        <v>2</v>
+      </c>
+      <c r="W22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="8:23" x14ac:dyDescent="0.2">
+      <c r="L23">
+        <v>2</v>
+      </c>
+      <c r="N23">
+        <v>5</v>
+      </c>
+      <c r="O23">
+        <v>1</v>
+      </c>
+      <c r="P23">
+        <v>6</v>
+      </c>
+      <c r="Q23">
+        <v>2</v>
+      </c>
+      <c r="R23">
+        <v>6</v>
+      </c>
+      <c r="S23">
+        <v>2</v>
+      </c>
+      <c r="T23">
+        <v>7</v>
+      </c>
+      <c r="U23">
+        <v>1</v>
+      </c>
+      <c r="W23">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="8:23" x14ac:dyDescent="0.2">
+      <c r="I24">
+        <v>1</v>
+      </c>
+      <c r="L24">
+        <v>1</v>
+      </c>
+      <c r="N24">
+        <v>4</v>
+      </c>
+      <c r="O24">
+        <v>2</v>
+      </c>
+      <c r="P24">
+        <v>8</v>
+      </c>
+      <c r="Q24">
+        <v>3</v>
+      </c>
+      <c r="R24">
+        <v>7</v>
+      </c>
+      <c r="S24">
+        <v>4</v>
+      </c>
+      <c r="T24">
+        <v>2</v>
+      </c>
+      <c r="U24">
+        <v>2</v>
+      </c>
+      <c r="W24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="8:23" x14ac:dyDescent="0.2">
+      <c r="I25">
+        <v>2</v>
+      </c>
+      <c r="L25">
+        <v>2</v>
+      </c>
+      <c r="M25">
+        <v>1</v>
+      </c>
+      <c r="N25">
+        <v>3</v>
+      </c>
+      <c r="O25">
+        <v>1</v>
+      </c>
+      <c r="P25">
+        <v>4</v>
+      </c>
+      <c r="Q25">
+        <v>2</v>
+      </c>
+      <c r="R25">
+        <v>8</v>
+      </c>
+      <c r="S25">
+        <v>6</v>
+      </c>
+      <c r="T25">
+        <v>8</v>
+      </c>
+      <c r="U25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="8:23" x14ac:dyDescent="0.2">
+      <c r="K26">
+        <v>1</v>
+      </c>
+      <c r="L26">
+        <v>3</v>
+      </c>
+      <c r="M26">
+        <v>2</v>
+      </c>
+      <c r="N26">
+        <v>2</v>
+      </c>
+      <c r="O26">
+        <v>2</v>
+      </c>
+      <c r="P26">
+        <v>8</v>
+      </c>
+      <c r="Q26">
+        <v>1</v>
+      </c>
+      <c r="R26">
+        <v>3</v>
+      </c>
+      <c r="S26">
+        <v>4</v>
+      </c>
+      <c r="T26">
+        <v>7</v>
+      </c>
+      <c r="U26">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="27" spans="8:23" x14ac:dyDescent="0.2">
+      <c r="I27">
+        <v>2</v>
+      </c>
+      <c r="L27">
+        <v>2</v>
+      </c>
+      <c r="M27">
+        <v>3</v>
+      </c>
+      <c r="N27">
+        <v>1</v>
+      </c>
+      <c r="O27">
+        <v>3</v>
+      </c>
+      <c r="P27">
+        <v>4</v>
+      </c>
+      <c r="Q27">
+        <v>2</v>
+      </c>
+      <c r="R27">
+        <v>8</v>
+      </c>
+      <c r="S27">
+        <v>6</v>
+      </c>
+      <c r="T27">
+        <v>2</v>
+      </c>
+      <c r="U27">
+        <v>3</v>
+      </c>
+      <c r="W27">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="8:23" x14ac:dyDescent="0.2">
+      <c r="H28">
+        <v>1</v>
+      </c>
+      <c r="J28">
+        <v>1</v>
+      </c>
+      <c r="L28">
+        <v>1</v>
+      </c>
+      <c r="M28">
+        <v>4</v>
+      </c>
+      <c r="O28">
+        <v>2</v>
+      </c>
+      <c r="P28">
+        <v>8</v>
+      </c>
+      <c r="Q28">
+        <v>3</v>
+      </c>
+      <c r="R28">
+        <v>3</v>
+      </c>
+      <c r="S28">
+        <v>4</v>
+      </c>
+      <c r="T28">
+        <v>7</v>
+      </c>
+      <c r="U28">
+        <v>2</v>
+      </c>
+      <c r="W28">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="29" spans="8:23" x14ac:dyDescent="0.2">
+      <c r="I29">
+        <v>2</v>
+      </c>
+      <c r="M29">
+        <v>5</v>
+      </c>
+      <c r="O29">
+        <v>1</v>
+      </c>
+      <c r="P29">
+        <v>6</v>
+      </c>
+      <c r="Q29">
+        <v>2</v>
+      </c>
+      <c r="R29">
+        <v>8</v>
+      </c>
+      <c r="S29">
+        <v>6</v>
+      </c>
+      <c r="T29">
+        <v>8</v>
+      </c>
+      <c r="U29">
+        <v>1</v>
+      </c>
+      <c r="W29">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="30" spans="8:23" x14ac:dyDescent="0.2">
+      <c r="L30">
+        <v>1</v>
+      </c>
+      <c r="M30">
+        <v>6</v>
+      </c>
+      <c r="P30">
+        <v>4</v>
+      </c>
+      <c r="Q30">
+        <v>1</v>
+      </c>
+      <c r="R30">
+        <v>3</v>
+      </c>
+      <c r="S30">
+        <v>4</v>
+      </c>
+      <c r="T30">
+        <v>2</v>
+      </c>
+      <c r="W30">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="31" spans="8:23" x14ac:dyDescent="0.2">
+      <c r="I31">
+        <v>2</v>
+      </c>
+      <c r="K31">
+        <v>1</v>
+      </c>
+      <c r="L31">
+        <v>2</v>
+      </c>
+      <c r="M31">
+        <v>7</v>
+      </c>
+      <c r="O31">
+        <v>1</v>
+      </c>
+      <c r="P31">
+        <v>2</v>
+      </c>
+      <c r="Q31">
+        <v>2</v>
+      </c>
+      <c r="R31">
+        <v>3</v>
+      </c>
+      <c r="S31">
+        <v>6</v>
+      </c>
+      <c r="T31">
+        <v>7</v>
+      </c>
+      <c r="W31">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="8:23" x14ac:dyDescent="0.2">
+      <c r="I32">
+        <v>1</v>
+      </c>
+      <c r="K32">
+        <v>2</v>
+      </c>
+      <c r="L32">
+        <v>3</v>
+      </c>
+      <c r="M32">
+        <v>8</v>
+      </c>
+      <c r="N32">
+        <v>1</v>
+      </c>
+      <c r="O32">
+        <v>1</v>
+      </c>
+      <c r="Q32">
+        <v>4</v>
+      </c>
+      <c r="R32">
+        <v>8</v>
+      </c>
+      <c r="S32">
+        <v>4</v>
+      </c>
+      <c r="T32">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="33" spans="8:23" x14ac:dyDescent="0.2">
+      <c r="H33">
+        <v>1</v>
+      </c>
+      <c r="K33">
+        <v>1</v>
+      </c>
+      <c r="L33">
+        <v>2</v>
+      </c>
+      <c r="M33">
+        <v>6</v>
+      </c>
+      <c r="N33">
+        <v>2</v>
+      </c>
+      <c r="Q33">
+        <v>6</v>
+      </c>
+      <c r="R33">
+        <v>3</v>
+      </c>
+      <c r="S33">
+        <v>2</v>
+      </c>
+      <c r="T33">
+        <v>5</v>
+      </c>
+      <c r="W33">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="8:23" x14ac:dyDescent="0.2">
+      <c r="H34">
+        <v>1</v>
+      </c>
+      <c r="L34">
+        <v>1</v>
+      </c>
+      <c r="M34">
+        <v>8</v>
+      </c>
+      <c r="N34">
+        <v>3</v>
+      </c>
+      <c r="Q34">
+        <v>6</v>
+      </c>
+      <c r="R34">
+        <v>2</v>
+      </c>
+      <c r="T34">
+        <v>4</v>
+      </c>
+      <c r="W34">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="35" spans="8:23" x14ac:dyDescent="0.2">
+      <c r="I35">
+        <v>1</v>
+      </c>
+      <c r="M35" s="5">
+        <v>6</v>
+      </c>
+      <c r="N35" s="5">
+        <v>4</v>
+      </c>
+      <c r="O35">
+        <v>1</v>
+      </c>
+      <c r="Q35">
+        <v>8</v>
+      </c>
+      <c r="R35">
+        <v>1</v>
+      </c>
+      <c r="S35" s="7">
+        <v>2</v>
+      </c>
+      <c r="T35">
+        <v>3</v>
+      </c>
+      <c r="W35">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="36" spans="8:23" x14ac:dyDescent="0.2">
+      <c r="I36">
+        <v>2</v>
+      </c>
+      <c r="L36">
+        <v>1</v>
+      </c>
+      <c r="M36" s="6">
+        <v>8</v>
+      </c>
+      <c r="N36" s="6">
+        <v>5</v>
+      </c>
+      <c r="O36">
+        <v>1</v>
+      </c>
+      <c r="P36">
+        <v>4</v>
+      </c>
+      <c r="Q36">
+        <v>3</v>
+      </c>
+      <c r="R36">
+        <v>2</v>
+      </c>
+      <c r="S36" s="8">
+        <v>4</v>
+      </c>
+      <c r="T36">
+        <v>2</v>
+      </c>
+      <c r="W36" s="5">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="37" spans="8:23" x14ac:dyDescent="0.2">
+      <c r="M37">
+        <v>6</v>
+      </c>
+      <c r="N37">
+        <v>4</v>
+      </c>
+      <c r="O37">
+        <v>1</v>
+      </c>
+      <c r="P37">
+        <v>6</v>
+      </c>
+      <c r="Q37">
+        <v>8</v>
+      </c>
+      <c r="R37">
+        <v>1</v>
+      </c>
+      <c r="S37" s="9">
+        <v>6</v>
+      </c>
+      <c r="T37">
+        <v>1</v>
+      </c>
+      <c r="W37" s="6">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="38" spans="8:23" x14ac:dyDescent="0.2">
+      <c r="L38">
+        <v>1</v>
+      </c>
+      <c r="M38">
+        <v>8</v>
+      </c>
+      <c r="N38">
+        <v>5</v>
+      </c>
+      <c r="P38">
+        <v>8</v>
+      </c>
+      <c r="Q38">
+        <v>3</v>
+      </c>
+      <c r="R38">
+        <v>1</v>
+      </c>
+      <c r="S38" s="8">
+        <v>4</v>
+      </c>
+      <c r="W38">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="39" spans="8:23" x14ac:dyDescent="0.2">
+      <c r="L39">
+        <v>2</v>
+      </c>
+      <c r="M39">
+        <v>7</v>
+      </c>
+      <c r="N39">
+        <v>4</v>
+      </c>
+      <c r="P39">
+        <v>4</v>
+      </c>
+      <c r="Q39">
+        <v>6</v>
+      </c>
+      <c r="S39" s="9">
+        <v>6</v>
+      </c>
+      <c r="W39">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="40" spans="8:23" x14ac:dyDescent="0.2">
+      <c r="L40">
+        <v>3</v>
+      </c>
+      <c r="M40">
+        <v>6</v>
+      </c>
+      <c r="N40">
+        <v>2</v>
+      </c>
+      <c r="O40">
+        <v>1</v>
+      </c>
+      <c r="P40">
+        <v>8</v>
+      </c>
+      <c r="Q40">
+        <v>6</v>
+      </c>
+      <c r="R40">
+        <v>1</v>
+      </c>
+      <c r="S40" s="8">
+        <v>4</v>
+      </c>
+      <c r="W40">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="41" spans="8:23" x14ac:dyDescent="0.2">
+      <c r="L41">
+        <v>2</v>
+      </c>
+      <c r="M41">
+        <v>5</v>
+      </c>
+      <c r="N41">
+        <v>4</v>
+      </c>
+      <c r="O41">
+        <v>2</v>
+      </c>
+      <c r="P41">
+        <v>4</v>
+      </c>
+      <c r="Q41">
+        <v>4</v>
+      </c>
+      <c r="R41">
+        <v>2</v>
+      </c>
+      <c r="S41" s="9">
+        <v>6</v>
+      </c>
+      <c r="T41">
+        <v>2</v>
+      </c>
+      <c r="W41">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="42" spans="8:23" x14ac:dyDescent="0.2">
+      <c r="L42">
+        <v>1</v>
+      </c>
+      <c r="M42">
+        <v>4</v>
+      </c>
+      <c r="N42">
+        <v>7</v>
+      </c>
+      <c r="O42">
+        <v>3</v>
+      </c>
+      <c r="P42">
+        <v>8</v>
+      </c>
+      <c r="Q42">
+        <v>2</v>
+      </c>
+      <c r="R42">
+        <v>1</v>
+      </c>
+      <c r="S42" s="8">
+        <v>4</v>
+      </c>
+      <c r="T42">
+        <v>4</v>
+      </c>
+      <c r="W42">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43" spans="8:23" x14ac:dyDescent="0.2">
+      <c r="L43">
+        <v>2</v>
+      </c>
+      <c r="M43">
+        <v>3</v>
+      </c>
+      <c r="N43">
+        <v>5</v>
+      </c>
+      <c r="O43">
+        <v>2</v>
+      </c>
+      <c r="P43">
+        <v>6</v>
+      </c>
+      <c r="Q43">
+        <v>1</v>
+      </c>
+      <c r="R43">
+        <v>2</v>
+      </c>
+      <c r="S43" s="9">
+        <v>6</v>
+      </c>
+      <c r="T43">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="44" spans="8:23" x14ac:dyDescent="0.2">
+      <c r="L44">
+        <v>3</v>
+      </c>
+      <c r="M44">
+        <v>2</v>
+      </c>
+      <c r="N44">
+        <v>7</v>
+      </c>
+      <c r="O44">
+        <v>1</v>
+      </c>
+      <c r="P44">
+        <v>4</v>
+      </c>
+      <c r="Q44">
+        <v>1</v>
+      </c>
+      <c r="R44">
+        <v>1</v>
+      </c>
+      <c r="S44" s="8">
+        <v>4</v>
+      </c>
+      <c r="T44">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="45" spans="8:23" x14ac:dyDescent="0.2">
+      <c r="L45">
+        <v>2</v>
+      </c>
+      <c r="M45">
+        <v>1</v>
+      </c>
+      <c r="N45">
+        <v>5</v>
+      </c>
+      <c r="P45">
+        <v>2</v>
+      </c>
+      <c r="R45">
+        <v>1</v>
+      </c>
+      <c r="S45" s="7">
+        <v>2</v>
+      </c>
+      <c r="T45">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="46" spans="8:23" x14ac:dyDescent="0.2">
+      <c r="L46">
+        <v>1</v>
+      </c>
+      <c r="N46">
+        <v>7</v>
+      </c>
+      <c r="R46">
+        <v>2</v>
+      </c>
+      <c r="S46">
+        <v>1</v>
+      </c>
+      <c r="T46">
+        <v>6</v>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="A1:XFD1048576">
-    <cfRule type="colorScale" priority="2">
+  <conditionalFormatting sqref="A35:L36 A1:XFD8 A9:L17 O9:XFD10 P11:XFD17 A47:XFD1048576 A37:N44 P35:R35 A45:O45 Q36:R44 T35:XFD40 A46:Q46 U41:XFD46 S46 Q45 W33:W35 W38:W41 A18:XFD34">
+    <cfRule type="containsBlanks" dxfId="10" priority="16">
+      <formula>LEN(TRIM(A1))=0</formula>
+    </cfRule>
+    <cfRule type="colorScale" priority="17">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -542,8 +1736,105 @@
         <color rgb="FFF5F0FF"/>
       </colorScale>
     </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A35:L36 A47:XFD1048576 A37:N44 P35:R35 A45:O45 Q36:R44 T35:XFD40 A46:Q46 U41:XFD46 S46 Q45 W33:W35 W38:W41 A1:XFD34">
+    <cfRule type="containsBlanks" dxfId="9" priority="15">
+      <formula>LEN(TRIM(A1))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="O35:O44">
+    <cfRule type="containsBlanks" dxfId="8" priority="13">
+      <formula>LEN(TRIM(O35))=0</formula>
+    </cfRule>
+    <cfRule type="colorScale" priority="14">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF4B317F"/>
+        <color rgb="FFAB7FFF"/>
+        <color rgb="FFF5F0FF"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="O35:O44">
+    <cfRule type="containsBlanks" dxfId="7" priority="12">
+      <formula>LEN(TRIM(O35))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="P36:P45">
+    <cfRule type="containsBlanks" dxfId="6" priority="10">
+      <formula>LEN(TRIM(P36))=0</formula>
+    </cfRule>
+    <cfRule type="colorScale" priority="11">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF4B317F"/>
+        <color rgb="FFAB7FFF"/>
+        <color rgb="FFF5F0FF"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="P36:P45">
+    <cfRule type="containsBlanks" dxfId="5" priority="9">
+      <formula>LEN(TRIM(P36))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="T41:T46">
+    <cfRule type="containsBlanks" dxfId="4" priority="7">
+      <formula>LEN(TRIM(T41))=0</formula>
+    </cfRule>
+    <cfRule type="colorScale" priority="8">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF4B317F"/>
+        <color rgb="FFAB7FFF"/>
+        <color rgb="FFF5F0FF"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="T41:T46">
+    <cfRule type="containsBlanks" dxfId="3" priority="6">
+      <formula>LEN(TRIM(T41))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="R45:R46">
+    <cfRule type="containsBlanks" dxfId="2" priority="4">
+      <formula>LEN(TRIM(R45))=0</formula>
+    </cfRule>
+    <cfRule type="colorScale" priority="5">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF4B317F"/>
+        <color rgb="FFAB7FFF"/>
+        <color rgb="FFF5F0FF"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="R45:R46">
+    <cfRule type="containsBlanks" dxfId="1" priority="3">
+      <formula>LEN(TRIM(R45))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A1:XFD1048576">
     <cfRule type="containsBlanks" dxfId="0" priority="1">
       <formula>LEN(TRIM(A1))=0</formula>
+    </cfRule>
+    <cfRule type="colorScale" priority="2">
+      <colorScale>
+        <cfvo type="num" val="1"/>
+        <cfvo type="num" val="4"/>
+        <cfvo type="num" val="8"/>
+        <color rgb="FF4B317F"/>
+        <color rgb="FFAB7FFF"/>
+        <color rgb="FFF5F0FF"/>
+      </colorScale>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Built test rig, added new animation strcat's for use in test classes
</commit_message>
<xml_diff>
--- a/animations/2-sparkle-a.xlsx
+++ b/animations/2-sparkle-a.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10410"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:11_{2B01B0BC-047F-E54A-BC44-CD08AD323A34}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6D0DB47-7AA1-8A44-9242-70FAE1404879}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="50240" windowHeight="28340" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="50220" windowHeight="28340" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -481,10 +481,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AT46"/>
+  <dimension ref="A1:W46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="400" zoomScaleNormal="400" workbookViewId="0">
-      <selection activeCell="J30" sqref="J30"/>
+    <sheetView tabSelected="1" zoomScale="400" zoomScaleNormal="400" workbookViewId="0">
+      <selection activeCell="C62" sqref="C62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -494,7 +494,7 @@
     <col min="22" max="46" width="2" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:46" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A1">
         <v>1</v>
       </c>
@@ -564,77 +564,8 @@
       <c r="W1">
         <v>3</v>
       </c>
-      <c r="X1">
-        <v>4</v>
-      </c>
-      <c r="Y1">
-        <v>5</v>
-      </c>
-      <c r="Z1">
-        <v>6</v>
-      </c>
-      <c r="AA1">
-        <v>7</v>
-      </c>
-      <c r="AB1">
-        <v>8</v>
-      </c>
-      <c r="AC1">
-        <v>9</v>
-      </c>
-      <c r="AD1">
-        <v>0</v>
-      </c>
-      <c r="AE1">
-        <v>1</v>
-      </c>
-      <c r="AF1">
-        <v>2</v>
-      </c>
-      <c r="AG1">
-        <v>3</v>
-      </c>
-      <c r="AH1">
-        <v>4</v>
-      </c>
-      <c r="AI1">
-        <v>5</v>
-      </c>
-      <c r="AJ1">
-        <v>6</v>
-      </c>
-      <c r="AK1">
-        <v>7</v>
-      </c>
-      <c r="AL1">
-        <v>8</v>
-      </c>
-      <c r="AM1">
-        <v>9</v>
-      </c>
-      <c r="AN1">
-        <v>0</v>
-      </c>
-      <c r="AO1">
-        <v>1</v>
-      </c>
-      <c r="AP1">
-        <v>2</v>
-      </c>
-      <c r="AQ1">
-        <v>3</v>
-      </c>
-      <c r="AR1">
-        <v>4</v>
-      </c>
-      <c r="AS1">
-        <v>5</v>
-      </c>
-      <c r="AT1">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="2" spans="1:46" x14ac:dyDescent="0.2">
+    </row>
+    <row r="2" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -663,7 +594,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:46" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:23" x14ac:dyDescent="0.2">
       <c r="B3">
         <v>1</v>
       </c>
@@ -692,7 +623,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:46" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:23" x14ac:dyDescent="0.2">
       <c r="C4">
         <v>1</v>
       </c>
@@ -721,7 +652,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:46" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:23" x14ac:dyDescent="0.2">
       <c r="E5">
         <v>1</v>
       </c>
@@ -747,7 +678,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:46" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:23" x14ac:dyDescent="0.2">
       <c r="F6">
         <v>1</v>
       </c>
@@ -770,7 +701,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:46" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:23" x14ac:dyDescent="0.2">
       <c r="H7">
         <v>1</v>
       </c>
@@ -790,7 +721,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:46" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:23" x14ac:dyDescent="0.2">
       <c r="I8">
         <v>1</v>
       </c>
@@ -807,7 +738,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="1:46" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:23" x14ac:dyDescent="0.2">
       <c r="K9">
         <v>1</v>
       </c>
@@ -821,7 +752,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="10" spans="1:46" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:23" x14ac:dyDescent="0.2">
       <c r="L10">
         <v>1</v>
       </c>
@@ -832,7 +763,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="1:46" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:23" x14ac:dyDescent="0.2">
       <c r="M11" s="2"/>
       <c r="N11" s="2">
         <v>1</v>
@@ -841,12 +772,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:46" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:23" x14ac:dyDescent="0.2">
       <c r="M12" s="2"/>
       <c r="N12" s="2"/>
       <c r="O12" s="2"/>
     </row>
-    <row r="13" spans="1:46" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:23" x14ac:dyDescent="0.2">
       <c r="M13" s="2"/>
       <c r="N13" s="2"/>
       <c r="O13" s="2"/>
@@ -854,7 +785,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:46" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:23" x14ac:dyDescent="0.2">
       <c r="M14" s="2"/>
       <c r="N14" s="2"/>
       <c r="O14" s="2"/>
@@ -865,7 +796,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:46" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:23" x14ac:dyDescent="0.2">
       <c r="M15" s="2"/>
       <c r="N15" s="2">
         <v>1</v>
@@ -881,7 +812,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="16" spans="1:46" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:23" x14ac:dyDescent="0.2">
       <c r="M16" s="2"/>
       <c r="N16" s="2">
         <v>1</v>

</xml_diff>